<commit_message>
added checklist to 4COM04_GenomeAssembly...
</commit_message>
<xml_diff>
--- a/templates/4COM04_GenomeAssembly/4COM04_GenomeAssembly.xlsx
+++ b/templates/4COM04_GenomeAssembly/4COM04_GenomeAssembly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/4COM04_GenomeAssembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0170423-4592-F249-8454-BD4991770AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1C00FD-4DCB-B54B-8901-4EF44AE16965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4680" yWindow="-21100" windowWidth="38360" windowHeight="21100" xr2:uid="{9EEB2079-C266-4F1B-B120-9813692A2E4B}"/>
   </bookViews>
@@ -979,7 +979,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F01384-B3A2-4F2D-B55D-8EA1341B1463}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AW30"/>
+  <dimension ref="A1:AT30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
       <selection activeCell="AR23" sqref="AR23"/>
@@ -2665,4 +2665,35 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<customXml>
+  <SwateTable Table="annotationTable" Worksheet="4COM04_GenomeAssembly">
+    <TableValidation DateTime="2021-06-09 14:32" SwateVersion="0.4.7" TableName="annotationTable" Userlist="" WorksheetName="4COM04_GenomeAssembly">
+      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="1" ColumnHeader="Sample Name" Importance="5" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="2" ColumnHeader="Parameter [BioSample Accession Number]" Importance="4" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="5" ColumnHeader="Parameter [Data filtering software]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="8" ColumnHeader="Parameter [Data filtering software version]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="11" ColumnHeader="Parameter [Data filtering Software Parameters]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="14" ColumnHeader="Parameter [Next generation sequencing instrument model]" Importance="5" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="17" ColumnHeader="Parameter [sequence assembly algorithm]" Importance="5" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="20" ColumnHeader="Parameter [Sequence assembly algorithm version]" Importance="4" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="23" ColumnHeader="Parameter [sequence assembly name]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="26" ColumnHeader="Parameter [genome coverage]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="29" ColumnHeader="Parameter [Genome status]" Importance="3" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="32" ColumnHeader="Parameter [Genome reference sequence]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="35" ColumnHeader="Parameter [Processed data file name]" Importance="5" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="38" ColumnHeader="Parameter [Processed data file format]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="41" ColumnHeader="Parameter [Processed data file checksum]" Importance="None" Unit="None" ValidationFormat="None"/>
+    </TableValidation>
+  </SwateTable>
+</customXml>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4DF26A5-A329-8145-A848-AC0BB93BE70D}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
</xml_diff>